<commit_message>
schematic updated to 0805 components and new usbcs
</commit_message>
<xml_diff>
--- a/Yun75_BoM.xlsx
+++ b/Yun75_BoM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Public\Documents\Altium\YunTKL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F2F8E79-E9BC-49CC-81CB-556F949DDF64}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBC4BD77-3657-43B1-86B0-9E27A7F65459}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30290" yWindow="2060" windowWidth="15530" windowHeight="15380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="18000" windowHeight="9457" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM Report" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="336">
   <si>
     <t>Bill of Materials</t>
   </si>
@@ -1025,6 +1025,18 @@
   </si>
   <si>
     <t>4-SMD, No Lead</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>Solder Joints/Part</t>
   </si>
 </sst>
 </file>
@@ -1524,7 +1536,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1920,6 +1932,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2199,27 +2219,29 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M69"/>
+  <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="13"/>
-    <col min="2" max="2" width="20.453125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="31.26953125" style="14" customWidth="1"/>
-    <col min="5" max="8" width="35.81640625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="36.453125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="10.54296875" style="13" customWidth="1"/>
-    <col min="11" max="12" width="9.1796875" style="13"/>
-    <col min="13" max="13" width="55.7265625" style="13" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="13"/>
+    <col min="1" max="1" width="9.19921875" style="13"/>
+    <col min="2" max="2" width="20.46484375" style="13" customWidth="1"/>
+    <col min="3" max="3" width="14.46484375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="31.265625" style="14" customWidth="1"/>
+    <col min="5" max="8" width="35.796875" style="13" customWidth="1"/>
+    <col min="9" max="9" width="36.46484375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="13" customWidth="1"/>
+    <col min="11" max="11" width="14.06640625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="10.53125" style="13" customWidth="1"/>
+    <col min="13" max="14" width="9.19921875" style="13"/>
+    <col min="15" max="15" width="55.73046875" style="13" customWidth="1"/>
+    <col min="16" max="16384" width="9.19921875" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:15">
       <c r="B1" s="15"/>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
@@ -2228,9 +2250,11 @@
       <c r="G1" s="17"/>
       <c r="H1" s="17"/>
       <c r="I1" s="17"/>
-      <c r="J1" s="18"/>
-    </row>
-    <row r="2" spans="1:13" ht="37.5" customHeight="1">
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="18"/>
+    </row>
+    <row r="2" spans="1:15" ht="37.5" customHeight="1">
       <c r="B2" s="19" t="s">
         <v>0</v>
       </c>
@@ -2243,9 +2267,11 @@
       <c r="G2" s="131"/>
       <c r="H2" s="131"/>
       <c r="I2" s="23"/>
-      <c r="J2" s="24"/>
-    </row>
-    <row r="3" spans="1:13" ht="23.25" customHeight="1">
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="24"/>
+    </row>
+    <row r="3" spans="1:15" ht="23.25" customHeight="1">
       <c r="B3" s="25" t="s">
         <v>2</v>
       </c>
@@ -2258,9 +2284,11 @@
       <c r="G3" s="27"/>
       <c r="H3" s="27"/>
       <c r="I3" s="28"/>
-      <c r="J3" s="29"/>
-    </row>
-    <row r="4" spans="1:13" ht="17.25" customHeight="1">
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="29"/>
+    </row>
+    <row r="4" spans="1:15" ht="17.25" customHeight="1">
       <c r="B4" s="25" t="s">
         <v>4</v>
       </c>
@@ -2273,9 +2301,11 @@
       <c r="G4" s="28"/>
       <c r="H4" s="28"/>
       <c r="I4" s="28"/>
-      <c r="J4" s="29"/>
-    </row>
-    <row r="5" spans="1:13" ht="17.25" customHeight="1">
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="29"/>
+    </row>
+    <row r="5" spans="1:15" ht="17.25" customHeight="1">
       <c r="B5" s="25" t="s">
         <v>6</v>
       </c>
@@ -2288,9 +2318,11 @@
       <c r="G5" s="28"/>
       <c r="H5" s="28"/>
       <c r="I5" s="28"/>
-      <c r="J5" s="29"/>
-    </row>
-    <row r="6" spans="1:13" ht="13">
+      <c r="J5" s="28"/>
+      <c r="K5" s="28"/>
+      <c r="L5" s="29"/>
+    </row>
+    <row r="6" spans="1:15" ht="13.15">
       <c r="B6" s="34"/>
       <c r="C6" s="32"/>
       <c r="D6" s="35"/>
@@ -2299,9 +2331,11 @@
       <c r="G6" s="33"/>
       <c r="H6" s="33"/>
       <c r="I6" s="36"/>
-      <c r="J6" s="37"/>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1">
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="37"/>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" customHeight="1">
       <c r="B7" s="38" t="s">
         <v>8</v>
       </c>
@@ -2316,28 +2350,32 @@
       <c r="G7" s="39"/>
       <c r="H7" s="39"/>
       <c r="I7" s="28"/>
-      <c r="J7" s="29"/>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1">
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="29"/>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" customHeight="1">
       <c r="B8" s="40" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="41">
         <f ca="1">TODAY()</f>
-        <v>43692</v>
+        <v>43694</v>
       </c>
       <c r="D8" s="42">
         <f ca="1">NOW()</f>
-        <v>43692.841096990742</v>
+        <v>43694.790478009258</v>
       </c>
       <c r="E8" s="39"/>
       <c r="F8" s="39"/>
       <c r="G8" s="39"/>
       <c r="H8" s="39"/>
       <c r="I8" s="28"/>
-      <c r="J8" s="29"/>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1">
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="29"/>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" customHeight="1">
       <c r="B9" s="38"/>
       <c r="C9" s="43"/>
       <c r="D9" s="43"/>
@@ -2346,9 +2384,11 @@
       <c r="G9" s="39"/>
       <c r="H9" s="39"/>
       <c r="I9" s="28"/>
-      <c r="J9" s="29"/>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1">
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="29"/>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" customHeight="1">
       <c r="B10" s="40"/>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
@@ -2357,12 +2397,14 @@
       <c r="G10" s="28"/>
       <c r="H10" s="28"/>
       <c r="I10" s="28"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="87"/>
-      <c r="M10" s="88"/>
-    </row>
-    <row r="11" spans="1:13" s="11" customFormat="1" ht="19.5" customHeight="1">
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="29"/>
+      <c r="M10" s="44"/>
+      <c r="N10" s="87"/>
+      <c r="O10" s="88"/>
+    </row>
+    <row r="11" spans="1:15" s="11" customFormat="1" ht="19.5" customHeight="1">
       <c r="A11" s="45" t="s">
         <v>12</v>
       </c>
@@ -2390,20 +2432,26 @@
       <c r="I11" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="48" t="s">
+      <c r="J11" s="46" t="s">
+        <v>332</v>
+      </c>
+      <c r="K11" s="46" t="s">
+        <v>335</v>
+      </c>
+      <c r="L11" s="48" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="49" t="s">
+      <c r="M11" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="L11" s="89" t="s">
+      <c r="N11" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="M11" s="88" t="s">
+      <c r="O11" s="88" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:13" s="12" customFormat="1" ht="16.5" customHeight="1">
+    <row r="12" spans="1:15" s="12" customFormat="1" ht="16.5" customHeight="1">
       <c r="A12" s="50" t="s">
         <v>22</v>
       </c>
@@ -2431,18 +2479,24 @@
       <c r="I12" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="53">
+      <c r="J12" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K12" s="50">
         <v>2</v>
       </c>
-      <c r="K12" s="54" t="s">
+      <c r="L12" s="53">
+        <v>2</v>
+      </c>
+      <c r="M12" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="L12" s="90" t="s">
+      <c r="N12" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M12" s="91"/>
-    </row>
-    <row r="13" spans="1:13" s="12" customFormat="1" ht="16.5" customHeight="1">
+      <c r="O12" s="91"/>
+    </row>
+    <row r="13" spans="1:15" s="12" customFormat="1" ht="16.5" customHeight="1">
       <c r="A13" s="50" t="s">
         <v>30</v>
       </c>
@@ -2470,18 +2524,24 @@
       <c r="I13" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="53">
+      <c r="J13" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K13" s="50">
+        <v>2</v>
+      </c>
+      <c r="L13" s="53">
         <v>88</v>
       </c>
-      <c r="K13" s="54" t="s">
+      <c r="M13" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="L13" s="90" t="s">
+      <c r="N13" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M13" s="91"/>
-    </row>
-    <row r="14" spans="1:13" s="12" customFormat="1" ht="16.5" customHeight="1">
+      <c r="O13" s="91"/>
+    </row>
+    <row r="14" spans="1:15" s="12" customFormat="1" ht="16.5" customHeight="1">
       <c r="A14" s="50" t="s">
         <v>36</v>
       </c>
@@ -2509,18 +2569,24 @@
       <c r="I14" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="J14" s="53">
+      <c r="J14" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K14" s="50">
         <v>2</v>
       </c>
-      <c r="K14" s="54" t="s">
+      <c r="L14" s="53">
+        <v>2</v>
+      </c>
+      <c r="M14" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="L14" s="90" t="s">
+      <c r="N14" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M14" s="91"/>
-    </row>
-    <row r="15" spans="1:13" ht="13">
+      <c r="O14" s="91"/>
+    </row>
+    <row r="15" spans="1:15" ht="13.15">
       <c r="A15" s="50" t="s">
         <v>43</v>
       </c>
@@ -2548,18 +2614,24 @@
       <c r="I15" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="J15" s="53">
+      <c r="J15" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K15" s="50">
         <v>2</v>
       </c>
-      <c r="K15" s="54" t="s">
+      <c r="L15" s="53">
+        <v>2</v>
+      </c>
+      <c r="M15" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="L15" s="90" t="s">
+      <c r="N15" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M15" s="91"/>
-    </row>
-    <row r="16" spans="1:13" customFormat="1" ht="13.75" customHeight="1">
+      <c r="O15" s="91"/>
+    </row>
+    <row r="16" spans="1:15" customFormat="1" ht="13.8" customHeight="1">
       <c r="A16" s="50" t="s">
         <v>46</v>
       </c>
@@ -2587,18 +2659,24 @@
       <c r="I16" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="J16" s="53">
+      <c r="J16" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K16" s="50">
+        <v>2</v>
+      </c>
+      <c r="L16" s="53">
         <v>1</v>
       </c>
-      <c r="K16" s="54" t="s">
+      <c r="M16" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L16" s="90" t="s">
+      <c r="N16" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M16" s="91"/>
-    </row>
-    <row r="17" spans="1:13" customFormat="1" ht="13" customHeight="1">
+      <c r="O16" s="91"/>
+    </row>
+    <row r="17" spans="1:15" customFormat="1" ht="13.05" customHeight="1">
       <c r="A17" s="50" t="s">
         <v>53</v>
       </c>
@@ -2626,18 +2704,24 @@
       <c r="I17" s="50" t="s">
         <v>56</v>
       </c>
-      <c r="J17" s="53">
+      <c r="J17" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K17" s="50">
+        <v>2</v>
+      </c>
+      <c r="L17" s="53">
         <v>1</v>
       </c>
-      <c r="K17" s="54" t="s">
+      <c r="M17" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L17" s="90" t="s">
+      <c r="N17" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M17" s="91"/>
-    </row>
-    <row r="18" spans="1:13" customFormat="1" ht="13" customHeight="1">
+      <c r="O17" s="91"/>
+    </row>
+    <row r="18" spans="1:15" customFormat="1" ht="13.05" customHeight="1">
       <c r="A18" s="50" t="s">
         <v>57</v>
       </c>
@@ -2665,18 +2749,24 @@
       <c r="I18" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="J18" s="53">
+      <c r="J18" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K18" s="50">
+        <v>2</v>
+      </c>
+      <c r="L18" s="53">
         <v>1</v>
       </c>
-      <c r="K18" s="54" t="s">
+      <c r="M18" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L18" s="90" t="s">
+      <c r="N18" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M18" s="91"/>
-    </row>
-    <row r="19" spans="1:13" customFormat="1" ht="13" customHeight="1">
+      <c r="O18" s="91"/>
+    </row>
+    <row r="19" spans="1:15" customFormat="1" ht="13.05" customHeight="1">
       <c r="A19" s="50" t="s">
         <v>62</v>
       </c>
@@ -2704,18 +2794,24 @@
       <c r="I19" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="J19" s="53">
+      <c r="J19" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K19" s="50">
+        <v>2</v>
+      </c>
+      <c r="L19" s="53">
         <v>1</v>
       </c>
-      <c r="K19" s="54" t="s">
+      <c r="M19" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L19" s="90" t="s">
+      <c r="N19" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M19" s="91"/>
-    </row>
-    <row r="20" spans="1:13" customFormat="1" ht="13" customHeight="1">
+      <c r="O19" s="91"/>
+    </row>
+    <row r="20" spans="1:15" customFormat="1" ht="13.05" customHeight="1">
       <c r="A20" s="50" t="s">
         <v>67</v>
       </c>
@@ -2743,18 +2839,24 @@
       <c r="I20" s="50" t="s">
         <v>72</v>
       </c>
-      <c r="J20" s="53">
+      <c r="J20" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K20" s="50">
+        <v>2</v>
+      </c>
+      <c r="L20" s="53">
         <v>1</v>
       </c>
-      <c r="K20" s="54" t="s">
+      <c r="M20" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L20" s="90" t="s">
+      <c r="N20" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M20" s="91"/>
-    </row>
-    <row r="21" spans="1:13" customFormat="1" ht="9.75" customHeight="1">
+      <c r="O20" s="91"/>
+    </row>
+    <row r="21" spans="1:15" customFormat="1" ht="9.75" customHeight="1">
       <c r="A21" s="50" t="s">
         <v>73</v>
       </c>
@@ -2782,18 +2884,24 @@
       <c r="I21" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="J21" s="53">
+      <c r="J21" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K21" s="50">
+        <v>2</v>
+      </c>
+      <c r="L21" s="53">
         <v>1</v>
       </c>
-      <c r="K21" s="54" t="s">
+      <c r="M21" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L21" s="90" t="s">
+      <c r="N21" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M21" s="91"/>
-    </row>
-    <row r="22" spans="1:13" customFormat="1" ht="13" customHeight="1">
+      <c r="O21" s="91"/>
+    </row>
+    <row r="22" spans="1:15" customFormat="1" ht="13.05" customHeight="1">
       <c r="A22" s="50" t="s">
         <v>78</v>
       </c>
@@ -2821,18 +2929,24 @@
       <c r="I22" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="J22" s="53">
+      <c r="J22" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K22" s="50">
+        <v>2</v>
+      </c>
+      <c r="L22" s="53">
         <v>84</v>
       </c>
-      <c r="K22" s="54" t="s">
+      <c r="M22" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="L22" s="90" t="s">
+      <c r="N22" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M22" s="91"/>
-    </row>
-    <row r="23" spans="1:13" customFormat="1" ht="13" customHeight="1">
+      <c r="O22" s="91"/>
+    </row>
+    <row r="23" spans="1:15" customFormat="1" ht="13.05" customHeight="1">
       <c r="A23" s="50" t="s">
         <v>84</v>
       </c>
@@ -2860,18 +2974,24 @@
       <c r="I23" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="J23" s="53">
+      <c r="J23" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K23" s="50">
+        <v>2</v>
+      </c>
+      <c r="L23" s="53">
         <v>1</v>
       </c>
-      <c r="K23" s="54" t="s">
+      <c r="M23" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L23" s="90" t="s">
+      <c r="N23" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M23" s="91"/>
-    </row>
-    <row r="24" spans="1:13" ht="13">
+      <c r="O23" s="91"/>
+    </row>
+    <row r="24" spans="1:15" ht="13.15">
       <c r="A24" s="50" t="s">
         <v>90</v>
       </c>
@@ -2899,18 +3019,24 @@
       <c r="I24" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="J24" s="53">
+      <c r="J24" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K24" s="50">
+        <v>2</v>
+      </c>
+      <c r="L24" s="53">
         <v>1</v>
       </c>
-      <c r="K24" s="54" t="s">
+      <c r="M24" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L24" s="90" t="s">
+      <c r="N24" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M24" s="91"/>
-    </row>
-    <row r="25" spans="1:13" ht="13">
+      <c r="O24" s="91"/>
+    </row>
+    <row r="25" spans="1:15" ht="13.15">
       <c r="A25" s="50" t="s">
         <v>96</v>
       </c>
@@ -2938,18 +3064,24 @@
       <c r="I25" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="J25" s="53">
+      <c r="J25" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K25" s="50">
+        <v>2</v>
+      </c>
+      <c r="L25" s="53">
         <v>1</v>
       </c>
-      <c r="K25" s="54" t="s">
+      <c r="M25" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L25" s="90" t="s">
+      <c r="N25" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M25" s="91"/>
-    </row>
-    <row r="26" spans="1:13" ht="13">
+      <c r="O25" s="91"/>
+    </row>
+    <row r="26" spans="1:15" ht="13.15">
       <c r="A26" s="50" t="s">
         <v>102</v>
       </c>
@@ -2977,18 +3109,24 @@
       <c r="I26" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="J26" s="53">
+      <c r="J26" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K26" s="50">
+        <v>2</v>
+      </c>
+      <c r="L26" s="53">
         <v>1</v>
       </c>
-      <c r="K26" s="54" t="s">
+      <c r="M26" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L26" s="90" t="s">
+      <c r="N26" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M26" s="91"/>
-    </row>
-    <row r="27" spans="1:13" ht="14">
+      <c r="O26" s="91"/>
+    </row>
+    <row r="27" spans="1:15" ht="13.5">
       <c r="A27" s="56" t="s">
         <v>107</v>
       </c>
@@ -3016,20 +3154,26 @@
       <c r="I27" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="J27" s="60">
+      <c r="J27" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K27" s="57">
+        <v>2</v>
+      </c>
+      <c r="L27" s="60">
         <v>3</v>
       </c>
-      <c r="K27" s="61" t="s">
+      <c r="M27" s="61" t="s">
         <v>112</v>
       </c>
-      <c r="L27" s="92" t="s">
+      <c r="N27" s="92" t="s">
         <v>113</v>
       </c>
-      <c r="M27" s="110" t="s">
+      <c r="O27" s="110" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="13">
+    <row r="28" spans="1:15" ht="13.15">
       <c r="A28" s="50" t="s">
         <v>114</v>
       </c>
@@ -3057,18 +3201,24 @@
       <c r="I28" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="J28" s="53">
+      <c r="J28" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K28" s="50">
+        <v>2</v>
+      </c>
+      <c r="L28" s="53">
         <v>1</v>
       </c>
-      <c r="K28" s="54" t="s">
+      <c r="M28" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L28" s="90" t="s">
+      <c r="N28" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M28" s="91"/>
-    </row>
-    <row r="29" spans="1:13" ht="13">
+      <c r="O28" s="91"/>
+    </row>
+    <row r="29" spans="1:15" ht="13.15">
       <c r="A29" s="50" t="s">
         <v>119</v>
       </c>
@@ -3094,18 +3244,24 @@
       <c r="I29" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="J29" s="53">
+      <c r="J29" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K29" s="50">
+        <v>24</v>
+      </c>
+      <c r="L29" s="53">
         <v>1</v>
       </c>
-      <c r="K29" s="54" t="s">
+      <c r="M29" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L29" s="90" t="s">
+      <c r="N29" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M29" s="91"/>
-    </row>
-    <row r="30" spans="1:13" ht="13">
+      <c r="O29" s="91"/>
+    </row>
+    <row r="30" spans="1:15" ht="13.15">
       <c r="A30" s="62" t="s">
         <v>124</v>
       </c>
@@ -3131,18 +3287,24 @@
       <c r="I30" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="J30" s="53">
+      <c r="J30" s="50" t="s">
+        <v>334</v>
+      </c>
+      <c r="K30" s="63">
+        <v>2</v>
+      </c>
+      <c r="L30" s="53">
         <v>1</v>
       </c>
-      <c r="K30" s="54" t="s">
+      <c r="M30" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L30" s="90" t="s">
+      <c r="N30" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M30" s="91"/>
-    </row>
-    <row r="31" spans="1:13" ht="13">
+      <c r="O30" s="91"/>
+    </row>
+    <row r="31" spans="1:15" ht="13.15">
       <c r="A31" s="50" t="s">
         <v>129</v>
       </c>
@@ -3170,18 +3332,24 @@
       <c r="I31" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="J31" s="53">
+      <c r="J31" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K31" s="50">
+        <v>2</v>
+      </c>
+      <c r="L31" s="53">
         <v>1</v>
       </c>
-      <c r="K31" s="54" t="s">
+      <c r="M31" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L31" s="90" t="s">
+      <c r="N31" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M31" s="91"/>
-    </row>
-    <row r="32" spans="1:13" ht="13">
+      <c r="O31" s="91"/>
+    </row>
+    <row r="32" spans="1:15" ht="13.15">
       <c r="A32" s="50" t="s">
         <v>134</v>
       </c>
@@ -3209,18 +3377,24 @@
       <c r="I32" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="J32" s="53">
+      <c r="J32" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K32" s="50">
+        <v>2</v>
+      </c>
+      <c r="L32" s="53">
         <v>1</v>
       </c>
-      <c r="K32" s="54" t="s">
+      <c r="M32" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L32" s="90" t="s">
+      <c r="N32" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M32" s="91"/>
-    </row>
-    <row r="33" spans="1:13" ht="13">
+      <c r="O32" s="91"/>
+    </row>
+    <row r="33" spans="1:15" ht="13.15">
       <c r="A33" s="50" t="s">
         <v>140</v>
       </c>
@@ -3248,18 +3422,24 @@
       <c r="I33" s="50" t="s">
         <v>145</v>
       </c>
-      <c r="J33" s="53">
+      <c r="J33" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K33" s="50">
         <v>2</v>
       </c>
-      <c r="K33" s="54" t="s">
+      <c r="L33" s="53">
+        <v>2</v>
+      </c>
+      <c r="M33" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="L33" s="90" t="s">
+      <c r="N33" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M33" s="91"/>
-    </row>
-    <row r="34" spans="1:13" ht="13">
+      <c r="O33" s="91"/>
+    </row>
+    <row r="34" spans="1:15" ht="13.15">
       <c r="A34" s="50" t="s">
         <v>146</v>
       </c>
@@ -3287,18 +3467,24 @@
       <c r="I34" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="J34" s="53">
+      <c r="J34" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K34" s="50">
         <v>2</v>
       </c>
-      <c r="K34" s="54" t="s">
+      <c r="L34" s="53">
+        <v>2</v>
+      </c>
+      <c r="M34" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="L34" s="90" t="s">
+      <c r="N34" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M34" s="91"/>
-    </row>
-    <row r="35" spans="1:13" ht="13">
+      <c r="O34" s="91"/>
+    </row>
+    <row r="35" spans="1:15" ht="13.15">
       <c r="A35" s="50" t="s">
         <v>151</v>
       </c>
@@ -3326,18 +3512,24 @@
       <c r="I35" s="50" t="s">
         <v>156</v>
       </c>
-      <c r="J35" s="53">
+      <c r="J35" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K35" s="50">
         <v>2</v>
       </c>
-      <c r="K35" s="54" t="s">
+      <c r="L35" s="53">
+        <v>2</v>
+      </c>
+      <c r="M35" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="L35" s="90" t="s">
+      <c r="N35" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M35" s="91"/>
-    </row>
-    <row r="36" spans="1:13" ht="13">
+      <c r="O35" s="91"/>
+    </row>
+    <row r="36" spans="1:15" ht="13.15">
       <c r="A36" s="50" t="s">
         <v>157</v>
       </c>
@@ -3365,18 +3557,24 @@
       <c r="I36" s="50" t="s">
         <v>160</v>
       </c>
-      <c r="J36" s="53">
+      <c r="J36" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K36" s="50">
+        <v>2</v>
+      </c>
+      <c r="L36" s="53">
         <v>4</v>
       </c>
-      <c r="K36" s="54" t="s">
+      <c r="M36" s="54" t="s">
         <v>161</v>
       </c>
-      <c r="L36" s="90" t="s">
+      <c r="N36" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M36" s="91"/>
-    </row>
-    <row r="37" spans="1:13" ht="13">
+      <c r="O36" s="91"/>
+    </row>
+    <row r="37" spans="1:15" ht="13.15">
       <c r="A37" s="50" t="s">
         <v>162</v>
       </c>
@@ -3404,18 +3602,24 @@
       <c r="I37" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="J37" s="53">
+      <c r="J37" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K37" s="50">
+        <v>2</v>
+      </c>
+      <c r="L37" s="53">
         <v>4</v>
       </c>
-      <c r="K37" s="54" t="s">
+      <c r="M37" s="54" t="s">
         <v>161</v>
       </c>
-      <c r="L37" s="90" t="s">
+      <c r="N37" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M37" s="91"/>
-    </row>
-    <row r="38" spans="1:13" ht="13">
+      <c r="O37" s="91"/>
+    </row>
+    <row r="38" spans="1:15" ht="13.15">
       <c r="A38" s="50" t="s">
         <v>167</v>
       </c>
@@ -3443,18 +3647,24 @@
       <c r="I38" s="50" t="s">
         <v>171</v>
       </c>
-      <c r="J38" s="53">
+      <c r="J38" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K38" s="50">
         <v>2</v>
       </c>
-      <c r="K38" s="54" t="s">
+      <c r="L38" s="53">
+        <v>2</v>
+      </c>
+      <c r="M38" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="L38" s="90" t="s">
+      <c r="N38" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M38" s="91"/>
-    </row>
-    <row r="39" spans="1:13" ht="13">
+      <c r="O38" s="91"/>
+    </row>
+    <row r="39" spans="1:15" ht="13.15">
       <c r="A39" s="50" t="s">
         <v>172</v>
       </c>
@@ -3482,18 +3692,24 @@
       <c r="I39" s="50" t="s">
         <v>176</v>
       </c>
-      <c r="J39" s="53">
+      <c r="J39" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K39" s="50">
+        <v>2</v>
+      </c>
+      <c r="L39" s="53">
         <v>3</v>
       </c>
-      <c r="K39" s="54" t="s">
+      <c r="M39" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="L39" s="90" t="s">
+      <c r="N39" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M39" s="91"/>
-    </row>
-    <row r="40" spans="1:13" ht="13">
+      <c r="O39" s="91"/>
+    </row>
+    <row r="40" spans="1:15" ht="13.15">
       <c r="A40" s="50" t="s">
         <v>177</v>
       </c>
@@ -3521,18 +3737,24 @@
       <c r="I40" s="50" t="s">
         <v>181</v>
       </c>
-      <c r="J40" s="53">
+      <c r="J40" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K40" s="50">
+        <v>2</v>
+      </c>
+      <c r="L40" s="53">
         <v>1</v>
       </c>
-      <c r="K40" s="54" t="s">
+      <c r="M40" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L40" s="90" t="s">
+      <c r="N40" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M40" s="91"/>
-    </row>
-    <row r="41" spans="1:13" ht="13">
+      <c r="O40" s="91"/>
+    </row>
+    <row r="41" spans="1:15" ht="13.15">
       <c r="A41" s="50" t="s">
         <v>182</v>
       </c>
@@ -3560,18 +3782,24 @@
       <c r="I41" s="50" t="s">
         <v>171</v>
       </c>
-      <c r="J41" s="53">
+      <c r="J41" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K41" s="50">
+        <v>2</v>
+      </c>
+      <c r="L41" s="53">
         <v>1</v>
       </c>
-      <c r="K41" s="54" t="s">
+      <c r="M41" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L41" s="90" t="s">
+      <c r="N41" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M41" s="91"/>
-    </row>
-    <row r="42" spans="1:13" ht="13">
+      <c r="O41" s="91"/>
+    </row>
+    <row r="42" spans="1:15" ht="13.15">
       <c r="A42" s="50" t="s">
         <v>184</v>
       </c>
@@ -3599,18 +3827,24 @@
       <c r="I42" s="50" t="s">
         <v>188</v>
       </c>
-      <c r="J42" s="53">
+      <c r="J42" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K42" s="50">
+        <v>2</v>
+      </c>
+      <c r="L42" s="53">
         <v>1</v>
       </c>
-      <c r="K42" s="54" t="s">
+      <c r="M42" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L42" s="90" t="s">
+      <c r="N42" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M42" s="91"/>
-    </row>
-    <row r="43" spans="1:13" ht="13">
+      <c r="O42" s="91"/>
+    </row>
+    <row r="43" spans="1:15" ht="13.15">
       <c r="A43" s="50" t="s">
         <v>189</v>
       </c>
@@ -3638,18 +3872,24 @@
       <c r="I43" s="50" t="s">
         <v>193</v>
       </c>
-      <c r="J43" s="53">
+      <c r="J43" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K43" s="50">
+        <v>2</v>
+      </c>
+      <c r="L43" s="53">
         <v>1</v>
       </c>
-      <c r="K43" s="54" t="s">
+      <c r="M43" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L43" s="90" t="s">
+      <c r="N43" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M43" s="91"/>
-    </row>
-    <row r="44" spans="1:13" ht="13">
+      <c r="O43" s="91"/>
+    </row>
+    <row r="44" spans="1:15" ht="13.15">
       <c r="A44" s="50" t="s">
         <v>194</v>
       </c>
@@ -3677,18 +3917,24 @@
       <c r="I44" s="50" t="s">
         <v>198</v>
       </c>
-      <c r="J44" s="53">
+      <c r="J44" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K44" s="50">
+        <v>2</v>
+      </c>
+      <c r="L44" s="53">
         <v>1</v>
       </c>
-      <c r="K44" s="54" t="s">
+      <c r="M44" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L44" s="90" t="s">
+      <c r="N44" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M44" s="91"/>
-    </row>
-    <row r="45" spans="1:13" ht="13">
+      <c r="O44" s="91"/>
+    </row>
+    <row r="45" spans="1:15" ht="13.15">
       <c r="A45" s="50" t="s">
         <v>199</v>
       </c>
@@ -3716,18 +3962,24 @@
       <c r="I45" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="J45" s="53">
+      <c r="J45" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K45" s="50">
+        <v>2</v>
+      </c>
+      <c r="L45" s="53">
         <v>1</v>
       </c>
-      <c r="K45" s="54" t="s">
+      <c r="M45" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L45" s="90" t="s">
+      <c r="N45" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M45" s="91"/>
-    </row>
-    <row r="46" spans="1:13" ht="13">
+      <c r="O45" s="91"/>
+    </row>
+    <row r="46" spans="1:15" ht="13.15">
       <c r="A46" s="50" t="s">
         <v>204</v>
       </c>
@@ -3753,18 +4005,24 @@
       <c r="I46" s="50" t="s">
         <v>208</v>
       </c>
-      <c r="J46" s="53">
+      <c r="J46" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K46" s="50">
+        <v>5</v>
+      </c>
+      <c r="L46" s="53">
         <v>1</v>
       </c>
-      <c r="K46" s="54" t="s">
+      <c r="M46" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L46" s="90" t="s">
+      <c r="N46" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M46" s="91"/>
-    </row>
-    <row r="47" spans="1:13" ht="13">
+      <c r="O46" s="91"/>
+    </row>
+    <row r="47" spans="1:15" ht="13.15">
       <c r="A47" s="50" t="s">
         <v>209</v>
       </c>
@@ -3790,18 +4048,24 @@
       <c r="I47" s="50" t="s">
         <v>213</v>
       </c>
-      <c r="J47" s="53">
+      <c r="J47" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K47" s="50">
+        <v>8</v>
+      </c>
+      <c r="L47" s="53">
         <v>1</v>
       </c>
-      <c r="K47" s="54" t="s">
+      <c r="M47" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L47" s="90" t="s">
+      <c r="N47" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M47" s="91"/>
-    </row>
-    <row r="48" spans="1:13" ht="13">
+      <c r="O47" s="91"/>
+    </row>
+    <row r="48" spans="1:15" ht="13.15">
       <c r="A48" s="50" t="s">
         <v>214</v>
       </c>
@@ -3827,18 +4091,24 @@
       <c r="I48" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="J48" s="53">
+      <c r="J48" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K48" s="50">
+        <v>2</v>
+      </c>
+      <c r="L48" s="53">
         <v>1</v>
       </c>
-      <c r="K48" s="54" t="s">
+      <c r="M48" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L48" s="90" t="s">
+      <c r="N48" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M48" s="91"/>
-    </row>
-    <row r="49" spans="1:13" ht="13">
+      <c r="O48" s="91"/>
+    </row>
+    <row r="49" spans="1:15" ht="13.15">
       <c r="A49" s="50" t="s">
         <v>219</v>
       </c>
@@ -3864,18 +4134,24 @@
       <c r="I49" s="50" t="s">
         <v>218</v>
       </c>
-      <c r="J49" s="53">
+      <c r="J49" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K49" s="50">
+        <v>4</v>
+      </c>
+      <c r="L49" s="53">
         <v>1</v>
       </c>
-      <c r="K49" s="54" t="s">
+      <c r="M49" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L49" s="90" t="s">
+      <c r="N49" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M49" s="91"/>
-    </row>
-    <row r="50" spans="1:13" ht="13">
+      <c r="O49" s="91"/>
+    </row>
+    <row r="50" spans="1:15" ht="13.15">
       <c r="A50" s="50" t="s">
         <v>223</v>
       </c>
@@ -3903,18 +4179,24 @@
       <c r="I50" s="50" t="s">
         <v>227</v>
       </c>
-      <c r="J50" s="53">
+      <c r="J50" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K50" s="50">
+        <v>44</v>
+      </c>
+      <c r="L50" s="53">
         <v>1</v>
       </c>
-      <c r="K50" s="54" t="s">
+      <c r="M50" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L50" s="90" t="s">
+      <c r="N50" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M50" s="91"/>
-    </row>
-    <row r="51" spans="1:13" ht="14">
+      <c r="O50" s="91"/>
+    </row>
+    <row r="51" spans="1:15" ht="13.5">
       <c r="A51" s="56" t="s">
         <v>228</v>
       </c>
@@ -3942,20 +4224,26 @@
       <c r="I51" s="57" t="s">
         <v>232</v>
       </c>
-      <c r="J51" s="60">
+      <c r="J51" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K51" s="57">
+        <v>5</v>
+      </c>
+      <c r="L51" s="60">
         <v>1</v>
       </c>
-      <c r="K51" s="61" t="s">
+      <c r="M51" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="L51" s="92" t="s">
+      <c r="N51" s="92" t="s">
         <v>113</v>
       </c>
-      <c r="M51" s="111" t="s">
+      <c r="O51" s="111" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="13">
+    <row r="52" spans="1:15" ht="13.15">
       <c r="A52" s="50" t="s">
         <v>233</v>
       </c>
@@ -3983,20 +4271,26 @@
       <c r="I52" s="50" t="s">
         <v>237</v>
       </c>
-      <c r="J52" s="53">
+      <c r="J52" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K52" s="50">
+        <v>3</v>
+      </c>
+      <c r="L52" s="53">
         <v>1</v>
       </c>
-      <c r="K52" s="54" t="s">
+      <c r="M52" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L52" s="90" t="s">
+      <c r="N52" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M52" s="132" t="s">
+      <c r="O52" s="132" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="13">
+    <row r="53" spans="1:15" ht="13.15">
       <c r="A53" s="50" t="s">
         <v>238</v>
       </c>
@@ -4024,18 +4318,24 @@
       <c r="I53" s="50" t="s">
         <v>237</v>
       </c>
-      <c r="J53" s="53">
+      <c r="J53" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K53" s="50">
+        <v>3</v>
+      </c>
+      <c r="L53" s="53">
         <v>1</v>
       </c>
-      <c r="K53" s="54" t="s">
+      <c r="M53" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L53" s="90" t="s">
+      <c r="N53" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M53" s="91"/>
-    </row>
-    <row r="54" spans="1:13" ht="13">
+      <c r="O53" s="91"/>
+    </row>
+    <row r="54" spans="1:15" ht="13.15">
       <c r="A54" s="67" t="s">
         <v>241</v>
       </c>
@@ -4063,20 +4363,26 @@
       <c r="I54" s="68" t="s">
         <v>245</v>
       </c>
-      <c r="J54" s="71">
+      <c r="J54" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K54" s="68">
+        <v>4</v>
+      </c>
+      <c r="L54" s="71">
         <v>1</v>
       </c>
-      <c r="K54" s="72" t="s">
+      <c r="M54" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="L54" s="93" t="s">
+      <c r="N54" s="93" t="s">
         <v>42</v>
       </c>
-      <c r="M54" s="109" t="s">
+      <c r="O54" s="109" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="13">
+    <row r="55" spans="1:15" ht="13.15">
       <c r="A55" s="50" t="s">
         <v>246</v>
       </c>
@@ -4104,18 +4410,24 @@
       <c r="I55" s="50" t="s">
         <v>250</v>
       </c>
-      <c r="J55" s="53">
+      <c r="J55" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K55" s="50">
+        <v>6</v>
+      </c>
+      <c r="L55" s="53">
         <v>1</v>
       </c>
-      <c r="K55" s="54" t="s">
+      <c r="M55" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L55" s="90" t="s">
+      <c r="N55" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M55" s="91"/>
-    </row>
-    <row r="56" spans="1:13" ht="13">
+      <c r="O55" s="91"/>
+    </row>
+    <row r="56" spans="1:15" ht="13.15">
       <c r="A56" s="50" t="s">
         <v>251</v>
       </c>
@@ -4143,18 +4455,24 @@
       <c r="I56" s="50" t="s">
         <v>255</v>
       </c>
-      <c r="J56" s="53">
+      <c r="J56" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K56" s="50">
+        <v>5</v>
+      </c>
+      <c r="L56" s="53">
         <v>1</v>
       </c>
-      <c r="K56" s="54" t="s">
+      <c r="M56" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L56" s="90" t="s">
+      <c r="N56" s="90" t="s">
         <v>29</v>
       </c>
-      <c r="M56" s="91"/>
-    </row>
-    <row r="57" spans="1:13" ht="13">
+      <c r="O56" s="91"/>
+    </row>
+    <row r="57" spans="1:15" ht="13.15">
       <c r="A57" s="50" t="s">
         <v>256</v>
       </c>
@@ -4182,18 +4500,24 @@
       <c r="I57" s="50" t="s">
         <v>260</v>
       </c>
-      <c r="J57" s="53">
+      <c r="J57" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K57" s="50">
+        <v>8</v>
+      </c>
+      <c r="L57" s="53">
         <v>1</v>
       </c>
-      <c r="K57" s="54" t="s">
+      <c r="M57" s="54" t="s">
         <v>52</v>
       </c>
-      <c r="L57" s="90" t="s">
+      <c r="N57" s="90" t="s">
         <v>42</v>
       </c>
-      <c r="M57" s="91"/>
-    </row>
-    <row r="58" spans="1:13" ht="13">
+      <c r="O57" s="91"/>
+    </row>
+    <row r="58" spans="1:15" ht="13.15">
       <c r="A58" s="113" t="s">
         <v>261</v>
       </c>
@@ -4221,18 +4545,24 @@
       <c r="I58" s="113" t="s">
         <v>266</v>
       </c>
-      <c r="J58" s="116">
+      <c r="J58" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K58" s="113">
+        <v>4</v>
+      </c>
+      <c r="L58" s="116">
         <v>1</v>
       </c>
-      <c r="K58" s="117">
+      <c r="M58" s="117">
         <v>5</v>
       </c>
-      <c r="L58" s="118" t="s">
+      <c r="N58" s="118" t="s">
         <v>42</v>
       </c>
-      <c r="M58" s="119"/>
-    </row>
-    <row r="59" spans="1:13" s="129" customFormat="1" ht="13">
+      <c r="O58" s="119"/>
+    </row>
+    <row r="59" spans="1:15" s="129" customFormat="1" ht="13.15">
       <c r="A59" s="112" t="s">
         <v>293</v>
       </c>
@@ -4260,14 +4590,20 @@
       <c r="I59" s="50" t="s">
         <v>297</v>
       </c>
-      <c r="J59" s="53">
+      <c r="J59" s="50" t="s">
+        <v>333</v>
+      </c>
+      <c r="K59" s="50">
+        <v>2</v>
+      </c>
+      <c r="L59" s="53">
         <v>1</v>
       </c>
-      <c r="K59" s="127"/>
-      <c r="L59" s="90"/>
-      <c r="M59" s="128"/>
-    </row>
-    <row r="60" spans="1:13">
+      <c r="M59" s="127"/>
+      <c r="N59" s="90"/>
+      <c r="O59" s="128"/>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60" s="12"/>
       <c r="B60" s="120"/>
       <c r="C60" s="121"/>
@@ -4277,12 +4613,14 @@
       <c r="G60" s="122"/>
       <c r="H60" s="122"/>
       <c r="I60" s="123"/>
-      <c r="J60" s="124">
-        <f>SUM(J12:J59)</f>
+      <c r="J60" s="123"/>
+      <c r="K60" s="123"/>
+      <c r="L60" s="124">
+        <f>SUM(L12:L59)</f>
         <v>235</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="13">
+    <row r="61" spans="1:15" ht="13.15">
       <c r="A61" s="12"/>
       <c r="B61" s="73" t="s">
         <v>267</v>
@@ -4296,9 +4634,11 @@
       <c r="G61" s="74"/>
       <c r="H61" s="133"/>
       <c r="I61" s="76"/>
-      <c r="J61" s="77"/>
-    </row>
-    <row r="62" spans="1:13">
+      <c r="J61" s="76"/>
+      <c r="K61" s="76"/>
+      <c r="L61" s="77"/>
+    </row>
+    <row r="62" spans="1:15">
       <c r="B62" s="78"/>
       <c r="C62" s="79"/>
       <c r="D62" s="80"/>
@@ -4307,9 +4647,11 @@
       <c r="G62" s="130"/>
       <c r="H62" s="130"/>
       <c r="I62" s="81"/>
-      <c r="J62" s="82"/>
-    </row>
-    <row r="63" spans="1:13">
+      <c r="J62" s="134"/>
+      <c r="K62" s="134"/>
+      <c r="L62" s="82"/>
+    </row>
+    <row r="63" spans="1:15">
       <c r="B63" s="83"/>
       <c r="C63" s="84"/>
       <c r="D63" s="85"/>
@@ -4318,9 +4660,11 @@
       <c r="G63" s="74"/>
       <c r="H63" s="74"/>
       <c r="I63" s="86"/>
-      <c r="J63" s="77"/>
-    </row>
-    <row r="64" spans="1:13">
+      <c r="J63" s="135"/>
+      <c r="K63" s="135"/>
+      <c r="L63" s="77"/>
+    </row>
+    <row r="64" spans="1:15">
       <c r="B64" s="83"/>
       <c r="C64" s="84"/>
       <c r="D64" s="85"/>
@@ -4329,9 +4673,11 @@
       <c r="G64" s="74"/>
       <c r="H64" s="74"/>
       <c r="I64" s="86"/>
-      <c r="J64" s="77"/>
-    </row>
-    <row r="65" spans="2:10">
+      <c r="J64" s="135"/>
+      <c r="K64" s="135"/>
+      <c r="L64" s="77"/>
+    </row>
+    <row r="65" spans="2:12">
       <c r="B65" s="83"/>
       <c r="C65" s="84"/>
       <c r="D65" s="85"/>
@@ -4340,9 +4686,11 @@
       <c r="G65" s="74"/>
       <c r="H65" s="74"/>
       <c r="I65" s="86"/>
-      <c r="J65" s="77"/>
-    </row>
-    <row r="66" spans="2:10">
+      <c r="J65" s="135"/>
+      <c r="K65" s="135"/>
+      <c r="L65" s="77"/>
+    </row>
+    <row r="66" spans="2:12">
       <c r="B66" s="94"/>
       <c r="C66" s="95"/>
       <c r="D66" s="96"/>
@@ -4351,9 +4699,11 @@
       <c r="G66" s="99"/>
       <c r="H66" s="99"/>
       <c r="I66" s="97"/>
-      <c r="J66" s="98"/>
-    </row>
-    <row r="67" spans="2:10">
+      <c r="J66" s="100"/>
+      <c r="K66" s="100"/>
+      <c r="L66" s="98"/>
+    </row>
+    <row r="67" spans="2:12">
       <c r="B67" s="94"/>
       <c r="C67" s="99"/>
       <c r="D67" s="99"/>
@@ -4362,9 +4712,11 @@
       <c r="G67" s="99"/>
       <c r="H67" s="99"/>
       <c r="I67" s="100"/>
-      <c r="J67" s="98"/>
-    </row>
-    <row r="68" spans="2:10" ht="13">
+      <c r="J67" s="100"/>
+      <c r="K67" s="100"/>
+      <c r="L67" s="98"/>
+    </row>
+    <row r="68" spans="2:12">
       <c r="B68" s="101"/>
       <c r="C68" s="102"/>
       <c r="D68" s="102"/>
@@ -4373,9 +4725,11 @@
       <c r="G68" s="102"/>
       <c r="H68" s="102"/>
       <c r="I68" s="103"/>
-      <c r="J68" s="104"/>
-    </row>
-    <row r="69" spans="2:10" ht="13">
+      <c r="J68" s="103"/>
+      <c r="K68" s="103"/>
+      <c r="L68" s="104"/>
+    </row>
+    <row r="69" spans="2:12">
       <c r="B69" s="105"/>
       <c r="C69" s="106"/>
       <c r="D69" s="106"/>
@@ -4384,7 +4738,9 @@
       <c r="G69" s="106"/>
       <c r="H69" s="106"/>
       <c r="I69" s="107"/>
-      <c r="J69" s="108"/>
+      <c r="J69" s="107"/>
+      <c r="K69" s="107"/>
+      <c r="L69" s="108"/>
     </row>
   </sheetData>
   <pageMargins left="0.45999999999999996" right="0.36" top="0.57999999999999996" bottom="1" header="0.5" footer="0.5"/>
@@ -4403,10 +4759,10 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="30.26953125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="108.54296875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="30.265625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="108.53125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="17.25" customHeight="1">

</xml_diff>